<commit_message>
Fix Enddate to 01.04.2020
</commit_message>
<xml_diff>
--- a/2020-03-21-Germany-Covid19-Prediction.xlsx
+++ b/2020-03-21-Germany-Covid19-Prediction.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -892,34 +892,6 @@
         <v>276989</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2">
-        <v>43921</v>
-      </c>
-      <c r="C32">
-        <v>30</v>
-      </c>
-      <c r="D32">
-        <v>361525</v>
-      </c>
-      <c r="E32">
-        <v>359248</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2">
-        <v>43922</v>
-      </c>
-      <c r="C33">
-        <v>31</v>
-      </c>
-      <c r="D33">
-        <v>469570</v>
-      </c>
-      <c r="E33">
-        <v>465736</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>